<commit_message>
Updates on cat results for semeval14 restaurant
</commit_message>
<xml_diff>
--- a/output/SemEval-14/Restaurants/agg.pred.eval.mean.20.0.0.xlsx
+++ b/output/SemEval-14/Restaurants/agg.pred.eval.mean.20.0.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hfani/Github/fani-lab/LADy/main/output/SemEval-14/Restaurants/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farinam\PycharmProjects\LADy\output\SemEval-14\Restaurants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4DCBED-5053-FB47-B395-771BC02F3812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE9C910-FA39-4DE0-BC5F-D30F31493DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="2" xr2:uid="{1230938A-22E1-464A-B275-4F8E3DAF70F5}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{1230938A-22E1-464A-B275-4F8E3DAF70F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -543,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -611,12 +611,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -934,16 +928,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F85FE2-0E4A-4FDA-8B9D-4C7A407A54D4}">
   <dimension ref="A1:I153"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="A133" sqref="A133:I153"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="A134" sqref="A134:I153"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -972,7 +966,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1001,7 +995,7 @@
         <v>0.192105263157894</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1030,7 +1024,7 @@
         <v>8.5526315789473506E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1059,7 +1053,7 @@
         <v>5.5657894736841997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1088,7 +1082,7 @@
         <v>1.1467105263157799E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1117,7 +1111,7 @@
         <v>0.114525375939849</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1146,7 +1140,7 @@
         <v>0.23855630653587701</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1175,7 +1169,7 @@
         <v>0.29961021598054099</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1204,7 +1198,7 @@
         <v>0.55901930623623797</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1233,7 +1227,7 @@
         <v>0.192105263157894</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1262,7 +1256,7 @@
         <v>0.20759023286387199</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1291,7 +1285,7 @@
         <v>0.229529939956577</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1320,7 +1314,7 @@
         <v>0.29357079993723301</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1349,7 +1343,7 @@
         <v>0.114525375939849</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1378,7 +1372,7 @@
         <v>0.16578640576554299</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1407,7 +1401,7 @@
         <v>0.175719236070385</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1436,7 +1430,7 @@
         <v>0.188284382665764</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1465,7 +1459,7 @@
         <v>0.192105263157894</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1494,7 +1488,7 @@
         <v>0.37302631578947298</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1523,7 +1517,7 @@
         <v>0.46447368421052598</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1552,7 +1546,7 @@
         <v>0.77565789473684199</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1581,7 +1575,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -1610,7 +1604,7 @@
         <v>0.24868421052631501</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -1639,7 +1633,7 @@
         <v>0.10328947368421</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1668,7 +1662,7 @@
         <v>6.2434210526315703E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1697,7 +1691,7 @@
         <v>1.21973684210525E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1726,7 +1720,7 @@
         <v>0.13715256897995801</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1755,7 +1749,7 @@
         <v>0.274053880387848</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1784,7 +1778,7 @@
         <v>0.324775909301532</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1813,7 +1807,7 @@
         <v>0.58298086426116102</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1842,7 +1836,7 @@
         <v>0.24868421052631501</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -1871,7 +1865,7 @@
         <v>0.248073422655502</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1900,7 +1894,7 @@
         <v>0.26561493234702799</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -1929,7 +1923,7 @@
         <v>0.33126830755069298</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -1958,7 +1952,7 @@
         <v>0.13715256897995801</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -1987,7 +1981,7 @@
         <v>0.19559457364318</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -2016,7 +2010,7 @@
         <v>0.20469629267005099</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -2045,7 +2039,7 @@
         <v>0.21849429484770799</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -2074,7 +2068,7 @@
         <v>0.24868421052631501</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -2103,7 +2097,7 @@
         <v>0.45394736842105199</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>20</v>
       </c>
@@ -2132,7 +2126,7 @@
         <v>0.51907894736842097</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>21</v>
       </c>
@@ -2161,7 +2155,7 @@
         <v>0.79539473684210504</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>1</v>
       </c>
@@ -2190,7 +2184,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -2219,7 +2213,7 @@
         <v>0.19934210526315699</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -2248,7 +2242,7 @@
         <v>0.103815789473684</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -2277,7 +2271,7 @@
         <v>6.6644736842105201E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -2306,7 +2300,7 @@
         <v>1.0809210526315701E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -2335,7 +2329,7 @@
         <v>0.123328895154553</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -2364,7 +2358,7 @@
         <v>0.29188482445147901</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -2393,7 +2387,7 @@
         <v>0.36307771896847302</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>9</v>
       </c>
@@ -2422,7 +2416,7 @@
         <v>0.54116844566636801</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -2451,7 +2445,7 @@
         <v>0.19934210526315699</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>11</v>
       </c>
@@ -2480,7 +2474,7 @@
         <v>0.244547326615594</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -2509,7 +2503,7 @@
         <v>0.27071162393861398</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>13</v>
       </c>
@@ -2538,7 +2532,7 @@
         <v>0.31859333977014698</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -2567,7 +2561,7 @@
         <v>0.123328895154553</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>15</v>
       </c>
@@ -2596,7 +2590,7 @@
         <v>0.19421831740352299</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>16</v>
       </c>
@@ -2625,7 +2619,7 @@
         <v>0.20657291727735499</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>17</v>
       </c>
@@ -2654,7 +2648,7 @@
         <v>0.21773795183281</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>18</v>
       </c>
@@ -2683,7 +2677,7 @@
         <v>0.19934210526315699</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>19</v>
       </c>
@@ -2712,7 +2706,7 @@
         <v>0.451315789473684</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>20</v>
       </c>
@@ -2741,7 +2735,7 @@
         <v>0.54276315789473595</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>21</v>
       </c>
@@ -2770,7 +2764,7 @@
         <v>0.75197368421052602</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>1</v>
       </c>
@@ -2799,7 +2793,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>2</v>
       </c>
@@ -2828,7 +2822,7 @@
         <v>7.1710526315789405E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>3</v>
       </c>
@@ -2857,7 +2851,7 @@
         <v>3.6447368421052603E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>4</v>
       </c>
@@ -2886,7 +2880,7 @@
         <v>2.60526315789473E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>5</v>
       </c>
@@ -2915,7 +2909,7 @@
         <v>7.8289473684209996E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>6</v>
       </c>
@@ -2944,7 +2938,7 @@
         <v>3.9450971177944799E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>7</v>
       </c>
@@ -2973,7 +2967,7 @@
         <v>9.7143330565248806E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -3002,7 +2996,7 @@
         <v>0.14074735263966501</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>9</v>
       </c>
@@ -3031,7 +3025,7 @@
         <v>0.38638084320650101</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>10</v>
       </c>
@@ -3060,7 +3054,7 @@
         <v>7.1710526315789405E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>11</v>
       </c>
@@ -3089,7 +3083,7 @@
         <v>8.1361926240573895E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>12</v>
       </c>
@@ -3118,7 +3112,7 @@
         <v>9.7132169677947702E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>13</v>
       </c>
@@ -3147,7 +3141,7 @@
         <v>0.15386294485994301</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>14</v>
       </c>
@@ -3176,7 +3170,7 @@
         <v>3.9450971177944799E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>15</v>
       </c>
@@ -3205,7 +3199,7 @@
         <v>6.13763537507045E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>16</v>
       </c>
@@ -3234,7 +3228,7 @@
         <v>6.8092234330894202E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>17</v>
       </c>
@@ -3263,7 +3257,7 @@
         <v>7.6910784646028393E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>18</v>
       </c>
@@ -3292,7 +3286,7 @@
         <v>7.1710526315789405E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>19</v>
       </c>
@@ -3321,7 +3315,7 @@
         <v>0.16578947368420999</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>20</v>
       </c>
@@ -3350,7 +3344,7 @@
         <v>0.230263157894736</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>21</v>
       </c>
@@ -3379,7 +3373,7 @@
         <v>0.58552631578947301</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>1</v>
       </c>
@@ -3408,7 +3402,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>2</v>
       </c>
@@ -3437,7 +3431,7 @@
         <v>1.3157894736842001E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>3</v>
       </c>
@@ -3466,7 +3460,7 @@
         <v>1.4605263157894699E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>4</v>
       </c>
@@ -3495,7 +3489,7 @@
         <v>1.8881578947368399E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>5</v>
       </c>
@@ -3524,7 +3518,7 @@
         <v>6.8026315789472998E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>6</v>
       </c>
@@ -3553,7 +3547,7 @@
         <v>1.012145748987E-4</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>7</v>
       </c>
@@ -3582,7 +3576,7 @@
         <v>3.5479919434212998E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>8</v>
       </c>
@@ -3611,7 +3605,7 @@
         <v>8.7976462115139306E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>9</v>
       </c>
@@ -3640,7 +3634,7 @@
         <v>0.30324846754123003</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>10</v>
       </c>
@@ -3669,7 +3663,7 @@
         <v>1.3157894736842001E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>11</v>
       </c>
@@ -3698,7 +3692,7 @@
         <v>1.9739058548339801E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>12</v>
       </c>
@@ -3727,7 +3721,7 @@
         <v>4.0207449662581898E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>13</v>
       </c>
@@ -3756,7 +3750,7 @@
         <v>9.3041857891330404E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>14</v>
       </c>
@@ -3785,7 +3779,7 @@
         <v>1.012145748987E-4</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>15</v>
       </c>
@@ -3814,7 +3808,7 @@
         <v>9.1839847594695004E-3</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>16</v>
       </c>
@@ -3843,7 +3837,7 @@
         <v>1.6739757807377499E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>17</v>
       </c>
@@ -3872,7 +3866,7 @@
         <v>2.58446236854178E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>18</v>
       </c>
@@ -3901,7 +3895,7 @@
         <v>1.3157894736842001E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>19</v>
       </c>
@@ -3930,7 +3924,7 @@
         <v>7.0394736842105204E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>20</v>
       </c>
@@ -3959,7 +3953,7 @@
         <v>0.17697368421052601</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>21</v>
       </c>
@@ -3988,7 +3982,7 @@
         <v>0.50657894736842102</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>1</v>
       </c>
@@ -4017,7 +4011,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>2</v>
       </c>
@@ -4046,7 +4040,7 @@
         <v>6.5789473684210004E-4</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>3</v>
       </c>
@@ -4075,7 +4069,7 @@
         <v>3.9473684210519999E-4</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>4</v>
       </c>
@@ -4104,7 +4098,7 @@
         <v>1.973684210526E-4</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>5</v>
       </c>
@@ -4133,7 +4127,7 @@
         <v>2.6315789473684198E-5</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>6</v>
       </c>
@@ -4162,7 +4156,7 @@
         <v>3.4626038781163397E-5</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>7</v>
       </c>
@@ -4191,7 +4185,7 @@
         <v>2.8133656509690002E-4</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>8</v>
       </c>
@@ -4220,7 +4214,7 @@
         <v>2.8133656509690002E-4</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>9</v>
       </c>
@@ -4249,7 +4243,7 @@
         <v>4.4581024930740002E-4</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>10</v>
       </c>
@@ -4278,7 +4272,7 @@
         <v>6.5789473684210004E-4</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>11</v>
       </c>
@@ -4307,7 +4301,7 @@
         <v>4.1858432456850001E-4</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>12</v>
       </c>
@@ -4336,7 +4330,7 @@
         <v>3.1582097180499999E-4</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>13</v>
       </c>
@@ -4365,7 +4359,7 @@
         <v>3.33331509043E-4</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>14</v>
       </c>
@@ -4394,7 +4388,7 @@
         <v>3.4626038781163397E-5</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>15</v>
       </c>
@@ -4423,7 +4417,7 @@
         <v>8.8079986149584404E-5</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>16</v>
       </c>
@@ -4452,7 +4446,7 @@
         <v>8.8079986149584404E-5</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>17</v>
       </c>
@@ -4481,7 +4475,7 @@
         <v>9.9828106450336305E-5</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>18</v>
       </c>
@@ -4510,7 +4504,7 @@
         <v>6.5789473684210004E-4</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>19</v>
       </c>
@@ -4539,7 +4533,7 @@
         <v>1.9736842105262998E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>20</v>
       </c>
@@ -4568,7 +4562,7 @@
         <v>1.9736842105262998E-3</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>21</v>
       </c>
@@ -4597,7 +4591,7 @@
         <v>2.6315789473684002E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>1</v>
       </c>
@@ -4626,111 +4620,111 @@
         <v>98</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>2</v>
       </c>
       <c r="B134">
-        <v>0.62920353982300892</v>
+        <v>0.34424778761061942</v>
       </c>
       <c r="C134">
-        <v>0.62300884955752212</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="D134">
-        <v>0.62743362831858396</v>
+        <v>0.62566371681415922</v>
       </c>
       <c r="E134">
-        <v>0.61946902654867253</v>
+        <v>0.61592920353982294</v>
       </c>
       <c r="F134">
-        <v>0.61946902654867253</v>
+        <v>0.61327433628318573</v>
       </c>
       <c r="G134">
-        <v>0.62035398230088501</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="H134">
-        <v>0.63274336283185839</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="I134">
-        <v>0.62300884955752212</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.63185840707964602</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>3</v>
       </c>
       <c r="B135">
-        <v>0.16814159292035391</v>
+        <v>0.1095575221238935</v>
       </c>
       <c r="C135">
-        <v>0.16495575221238931</v>
+        <v>0.1653097345132743</v>
       </c>
       <c r="D135">
-        <v>0.16707964601769909</v>
+        <v>0.1672566371681416</v>
       </c>
       <c r="E135">
-        <v>0.1656637168141592</v>
+        <v>0.16548672566371669</v>
       </c>
       <c r="F135">
-        <v>0.16424778761061939</v>
+        <v>0.16318584070796449</v>
       </c>
       <c r="G135">
         <v>0.16495575221238931</v>
       </c>
       <c r="H135">
-        <v>0.16690265486725661</v>
+        <v>0.16707964601769909</v>
       </c>
       <c r="I135">
-        <v>0.16353982300884939</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.1647787610619468</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>4</v>
       </c>
       <c r="B136">
-        <v>8.5132743362831803E-2</v>
+        <v>6.4513274336282997E-2</v>
       </c>
       <c r="C136">
-        <v>8.3716814159291997E-2</v>
+        <v>8.3893805309734504E-2</v>
       </c>
       <c r="D136">
-        <v>8.4867256637168098E-2</v>
+        <v>8.44247787610619E-2</v>
       </c>
       <c r="E136">
-        <v>8.3893805309734504E-2</v>
+        <v>8.3628318584070799E-2</v>
       </c>
       <c r="F136">
-        <v>8.3628318584070799E-2</v>
+        <v>8.3539823008849504E-2</v>
       </c>
       <c r="G136">
-        <v>8.3716814159291997E-2</v>
+        <v>8.3805309734513195E-2</v>
       </c>
       <c r="H136">
-        <v>8.4513274336283098E-2</v>
+        <v>8.4690265486725605E-2</v>
       </c>
       <c r="I136">
-        <v>8.3097345132743305E-2</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+        <v>8.3362831858406997E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>5</v>
       </c>
       <c r="B137">
-        <v>8.7433628318583992E-3</v>
+        <v>8.4424778761062001E-3</v>
       </c>
       <c r="C137">
+        <v>8.6814159292035002E-3</v>
+      </c>
+      <c r="D137">
         <v>8.6460176991149992E-3</v>
       </c>
-      <c r="D137">
-        <v>8.6637168141592003E-3</v>
-      </c>
       <c r="E137">
-        <v>8.6283185840707998E-3</v>
+        <v>8.6371681415928995E-3</v>
       </c>
       <c r="F137">
-        <v>8.7079646017698999E-3</v>
+        <v>8.6725663716814005E-3</v>
       </c>
       <c r="G137">
         <v>8.6548672566371006E-3</v>
@@ -4739,114 +4733,114 @@
         <v>8.6548672566371006E-3</v>
       </c>
       <c r="I137">
-        <v>8.6017699115044002E-3</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+        <v>8.6460176991149992E-3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>6</v>
       </c>
       <c r="B138">
-        <v>0.62920353982300892</v>
+        <v>0.34424778761061942</v>
       </c>
       <c r="C138">
-        <v>0.62300884955752212</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="D138">
-        <v>0.62743362831858396</v>
+        <v>0.62566371681415922</v>
       </c>
       <c r="E138">
-        <v>0.61946902654867253</v>
+        <v>0.61592920353982294</v>
       </c>
       <c r="F138">
-        <v>0.61946902654867253</v>
+        <v>0.61327433628318573</v>
       </c>
       <c r="G138">
-        <v>0.62035398230088501</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="H138">
-        <v>0.63274336283185839</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="I138">
-        <v>0.62300884955752212</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.63185840707964602</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>7</v>
       </c>
       <c r="B139">
-        <v>0.84070796460176989</v>
+        <v>0.54778761061946901</v>
       </c>
       <c r="C139">
-        <v>0.82477876106194681</v>
+        <v>0.82654867256637166</v>
       </c>
       <c r="D139">
-        <v>0.83539823008849545</v>
+        <v>0.83628318584070782</v>
       </c>
       <c r="E139">
-        <v>0.82831858407079628</v>
+        <v>0.82743362831858391</v>
       </c>
       <c r="F139">
-        <v>0.82123893805309733</v>
+        <v>0.81592920353982312</v>
       </c>
       <c r="G139">
         <v>0.82477876106194681</v>
       </c>
       <c r="H139">
-        <v>0.8345132743362832</v>
+        <v>0.83539823008849567</v>
       </c>
       <c r="I139">
-        <v>0.81769911504424775</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.82389380530973444</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>8</v>
       </c>
       <c r="B140">
-        <v>0.85132743362831853</v>
+        <v>0.64513274336283177</v>
       </c>
       <c r="C140">
-        <v>0.8371681415929203</v>
+        <v>0.83893805309734515</v>
       </c>
       <c r="D140">
-        <v>0.84867256637168142</v>
+        <v>0.84424778761061958</v>
       </c>
       <c r="E140">
-        <v>0.83893805309734515</v>
+        <v>0.83628318584070782</v>
       </c>
       <c r="F140">
-        <v>0.83628318584070804</v>
+        <v>0.83539823008849567</v>
       </c>
       <c r="G140">
-        <v>0.8371681415929203</v>
+        <v>0.83805309734513267</v>
       </c>
       <c r="H140">
-        <v>0.84513274336283184</v>
+        <v>0.84690265486725669</v>
       </c>
       <c r="I140">
-        <v>0.83097345132743372</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.83362831858407083</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>9</v>
       </c>
       <c r="B141">
-        <v>0.87433628318584078</v>
+        <v>0.84424778761061936</v>
       </c>
       <c r="C141">
+        <v>0.86814159292035398</v>
+      </c>
+      <c r="D141">
         <v>0.86460176991150439</v>
       </c>
-      <c r="D141">
-        <v>0.86637168141592924</v>
-      </c>
       <c r="E141">
-        <v>0.86283185840707977</v>
+        <v>0.86371681415929191</v>
       </c>
       <c r="F141">
-        <v>0.87079646017699108</v>
+        <v>0.86725663716814161</v>
       </c>
       <c r="G141">
         <v>0.86548672566371676</v>
@@ -4855,346 +4849,346 @@
         <v>0.86548672566371676</v>
       </c>
       <c r="I141">
-        <v>0.86017699115044244</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.8646017699115045</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>10</v>
       </c>
       <c r="B142">
-        <v>0.62920353982300892</v>
+        <v>0.34424778761061942</v>
       </c>
       <c r="C142">
-        <v>0.62300884955752212</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="D142">
-        <v>0.62743362831858396</v>
+        <v>0.62566371681415922</v>
       </c>
       <c r="E142">
-        <v>0.61946902654867253</v>
+        <v>0.61592920353982294</v>
       </c>
       <c r="F142">
-        <v>0.61946902654867253</v>
+        <v>0.61327433628318573</v>
       </c>
       <c r="G142">
-        <v>0.62035398230088501</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="H142">
-        <v>0.63274336283185839</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="I142">
-        <v>0.62300884955752212</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.63185840707964602</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>11</v>
       </c>
       <c r="B143">
-        <v>0.75223240980849693</v>
+        <v>0.45191435477082248</v>
       </c>
       <c r="C143">
-        <v>0.7415343956944036</v>
+        <v>0.74167904013767016</v>
       </c>
       <c r="D143">
-        <v>0.74921276764635736</v>
+        <v>0.74872040639660964</v>
       </c>
       <c r="E143">
-        <v>0.74143207160270697</v>
+        <v>0.73992854309119571</v>
       </c>
       <c r="F143">
-        <v>0.73728826916094825</v>
+        <v>0.73212857139942233</v>
       </c>
       <c r="G143">
-        <v>0.73909805936333373</v>
+        <v>0.73948967234156338</v>
       </c>
       <c r="H143">
-        <v>0.75075982941528285</v>
+        <v>0.7500509685462633</v>
       </c>
       <c r="I143">
-        <v>0.73668125318101874</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.74347147090489041</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>12</v>
       </c>
       <c r="B144">
-        <v>0.75565007805945172</v>
+        <v>0.4834295304997836</v>
       </c>
       <c r="C144">
-        <v>0.7458116242261299</v>
+        <v>0.74570371874480279</v>
       </c>
       <c r="D144">
-        <v>0.75361302681350373</v>
+        <v>0.75129300719245173</v>
       </c>
       <c r="E144">
-        <v>0.74491872960937111</v>
+        <v>0.7429352075230452</v>
       </c>
       <c r="F144">
-        <v>0.74232327273207699</v>
+        <v>0.73842433237667227</v>
       </c>
       <c r="G144">
-        <v>0.74321829309646603</v>
+        <v>0.74378386970299437</v>
       </c>
       <c r="H144">
-        <v>0.75441276183895867</v>
+        <v>0.75385285415213787</v>
       </c>
       <c r="I144">
-        <v>0.74110394028228066</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.74684219230890991</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>13</v>
       </c>
       <c r="B145">
-        <v>0.76030110285253905</v>
+        <v>0.52517248409274941</v>
       </c>
       <c r="C145">
-        <v>0.75128517689708219</v>
+        <v>0.75113363554325607</v>
       </c>
       <c r="D145">
-        <v>0.75724205476213735</v>
+        <v>0.75569324226199253</v>
       </c>
       <c r="E145">
-        <v>0.74978408834054755</v>
+        <v>0.74839396494972288</v>
       </c>
       <c r="F145">
-        <v>0.74946048218436134</v>
+        <v>0.74470896382332741</v>
       </c>
       <c r="G145">
-        <v>0.74882371759365562</v>
+        <v>0.7492237815007089</v>
       </c>
       <c r="H145">
-        <v>0.75850986732845715</v>
+        <v>0.75731407461203493</v>
       </c>
       <c r="I145">
-        <v>0.74677607454431738</v>
-      </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.75271844974994939</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>14</v>
       </c>
       <c r="B146">
-        <v>0.62920353982300892</v>
+        <v>0.34424778761061942</v>
       </c>
       <c r="C146">
-        <v>0.62300884955752212</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="D146">
-        <v>0.62743362831858396</v>
+        <v>0.62566371681415922</v>
       </c>
       <c r="E146">
-        <v>0.61946902654867253</v>
+        <v>0.61592920353982294</v>
       </c>
       <c r="F146">
-        <v>0.61946902654867253</v>
+        <v>0.61327433628318573</v>
       </c>
       <c r="G146">
-        <v>0.62035398230088501</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="H146">
-        <v>0.63274336283185839</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="I146">
-        <v>0.62300884955752212</v>
-      </c>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.63185840707964602</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>15</v>
       </c>
       <c r="B147">
-        <v>0.72185840707964599</v>
+        <v>0.42007374631268429</v>
       </c>
       <c r="C147">
-        <v>0.71280235988200591</v>
+        <v>0.71246312684365765</v>
       </c>
       <c r="D147">
-        <v>0.71952802359881995</v>
+        <v>0.71861356932153397</v>
       </c>
       <c r="E147">
-        <v>0.71154867256637166</v>
+        <v>0.70977876106194693</v>
       </c>
       <c r="F147">
-        <v>0.70839233038348071</v>
+        <v>0.70324483775811208</v>
       </c>
       <c r="G147">
-        <v>0.70966076696165181</v>
+        <v>0.71023598820058997</v>
       </c>
       <c r="H147">
-        <v>0.72190265486725658</v>
+        <v>0.72072271386430675</v>
       </c>
       <c r="I147">
-        <v>0.70877581120943955</v>
-      </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.71584070796460164</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>16</v>
       </c>
       <c r="B148">
-        <v>0.72325677763730856</v>
+        <v>0.43310226155358889</v>
       </c>
       <c r="C148">
-        <v>0.71472924568057306</v>
+        <v>0.71413681696867537</v>
       </c>
       <c r="D148">
-        <v>0.72140679870768365</v>
+        <v>0.71967376035960107</v>
       </c>
       <c r="E148">
-        <v>0.71301973591796597</v>
+        <v>0.71110443882567775</v>
       </c>
       <c r="F148">
-        <v>0.7105734653743504</v>
+        <v>0.70584211265627195</v>
       </c>
       <c r="G148">
-        <v>0.71142786908273625</v>
+        <v>0.71200906026127275</v>
       </c>
       <c r="H148">
-        <v>0.7235391206630144</v>
+        <v>0.72234126984126967</v>
       </c>
       <c r="I148">
-        <v>0.71067811490377863</v>
-      </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.71736304256215755</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>17</v>
       </c>
       <c r="B149">
-        <v>0.72413532427085325</v>
+        <v>0.44137392430668798</v>
       </c>
       <c r="C149">
-        <v>0.71570067085624189</v>
+        <v>0.71493795019210093</v>
       </c>
       <c r="D149">
-        <v>0.72209482924078139</v>
+        <v>0.72059889693637558</v>
       </c>
       <c r="E149">
-        <v>0.71394505844708278</v>
+        <v>0.7120941084865916</v>
       </c>
       <c r="F149">
-        <v>0.71195529433083737</v>
+        <v>0.70689506514116796</v>
       </c>
       <c r="G149">
-        <v>0.71240030930980858</v>
+        <v>0.71298017721829265</v>
       </c>
       <c r="H149">
-        <v>0.72425221734611522</v>
+        <v>0.72285130294618338</v>
       </c>
       <c r="I149">
-        <v>0.71162156178649771</v>
-      </c>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.71827337168777072</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>18</v>
       </c>
       <c r="B150">
-        <v>0.62920353982300892</v>
+        <v>0.34424778761061942</v>
       </c>
       <c r="C150">
-        <v>0.62300884955752212</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="D150">
-        <v>0.62743362831858396</v>
+        <v>0.62566371681415922</v>
       </c>
       <c r="E150">
-        <v>0.61946902654867253</v>
+        <v>0.61592920353982294</v>
       </c>
       <c r="F150">
-        <v>0.61946902654867253</v>
+        <v>0.61327433628318573</v>
       </c>
       <c r="G150">
-        <v>0.62035398230088501</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="H150">
-        <v>0.63274336283185839</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="I150">
-        <v>0.62300884955752212</v>
-      </c>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.63185840707964602</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>19</v>
       </c>
       <c r="B151">
-        <v>0.84070796460176989</v>
+        <v>0.54778761061946901</v>
       </c>
       <c r="C151">
-        <v>0.82477876106194681</v>
+        <v>0.82654867256637166</v>
       </c>
       <c r="D151">
-        <v>0.83539823008849545</v>
+        <v>0.83628318584070782</v>
       </c>
       <c r="E151">
-        <v>0.82831858407079628</v>
+        <v>0.82743362831858391</v>
       </c>
       <c r="F151">
-        <v>0.82123893805309733</v>
+        <v>0.81592920353982312</v>
       </c>
       <c r="G151">
         <v>0.82477876106194681</v>
       </c>
       <c r="H151">
-        <v>0.8345132743362832</v>
+        <v>0.83539823008849567</v>
       </c>
       <c r="I151">
-        <v>0.81769911504424775</v>
-      </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.82389380530973444</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>20</v>
       </c>
       <c r="B152">
-        <v>0.85132743362831853</v>
+        <v>0.64513274336283177</v>
       </c>
       <c r="C152">
-        <v>0.8371681415929203</v>
+        <v>0.83893805309734515</v>
       </c>
       <c r="D152">
-        <v>0.84867256637168142</v>
+        <v>0.84424778761061958</v>
       </c>
       <c r="E152">
-        <v>0.83893805309734515</v>
+        <v>0.83628318584070782</v>
       </c>
       <c r="F152">
-        <v>0.83628318584070804</v>
+        <v>0.83539823008849567</v>
       </c>
       <c r="G152">
-        <v>0.8371681415929203</v>
+        <v>0.83805309734513267</v>
       </c>
       <c r="H152">
-        <v>0.84513274336283184</v>
+        <v>0.84690265486725669</v>
       </c>
       <c r="I152">
-        <v>0.83097345132743372</v>
-      </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.83362831858407083</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>21</v>
       </c>
       <c r="B153">
-        <v>0.87433628318584078</v>
+        <v>0.84424778761061936</v>
       </c>
       <c r="C153">
+        <v>0.86814159292035398</v>
+      </c>
+      <c r="D153">
         <v>0.86460176991150439</v>
       </c>
-      <c r="D153">
-        <v>0.86637168141592924</v>
-      </c>
       <c r="E153">
-        <v>0.86283185840707977</v>
+        <v>0.86371681415929191</v>
       </c>
       <c r="F153">
-        <v>0.87079646017699108</v>
+        <v>0.86725663716814161</v>
       </c>
       <c r="G153">
         <v>0.86548672566371676</v>
@@ -5203,7 +5197,7 @@
         <v>0.86548672566371676</v>
       </c>
       <c r="I153">
-        <v>0.86017699115044244</v>
+        <v>0.8646017699115045</v>
       </c>
     </row>
   </sheetData>
@@ -5216,15 +5210,15 @@
   <dimension ref="A1:CJ107"/>
   <sheetViews>
     <sheetView topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M89" sqref="M89"/>
+      <selection activeCell="B88" sqref="B88:I107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -5341,7 +5335,7 @@
       <c r="CI1" s="19"/>
       <c r="CJ1" s="19"/>
     </row>
-    <row r="2" spans="1:88" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -5601,7 +5595,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:88" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -5861,7 +5855,7 @@
         <v>1.0599415204669999E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:88" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -6121,7 +6115,7 @@
         <v>2.861379300524E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:88" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -6381,7 +6375,7 @@
         <v>6.4068591617929996E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:88" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -6641,7 +6635,7 @@
         <v>4.2847188634349999E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:88" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -6901,7 +6895,7 @@
         <v>1.3706140350870001E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:88" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -7161,7 +7155,7 @@
         <v>1.4363535433480001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:88" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -7421,7 +7415,7 @@
         <v>2.1076998050679999E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:88" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -7681,7 +7675,7 @@
         <v>8.8079986149584404E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:88" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -7710,7 +7704,7 @@
         <v>0.114525375939849</v>
       </c>
     </row>
-    <row r="12" spans="1:88" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -7739,7 +7733,7 @@
         <v>0.16578640576554299</v>
       </c>
     </row>
-    <row r="13" spans="1:88" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -7768,7 +7762,7 @@
         <v>0.175719236070385</v>
       </c>
     </row>
-    <row r="15" spans="1:88" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -7797,7 +7791,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:88" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -7826,7 +7820,7 @@
         <v>0.24868421052631501</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -7855,7 +7849,7 @@
         <v>0.10328947368421</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -7884,7 +7878,7 @@
         <v>6.2434210526315703E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -7913,7 +7907,7 @@
         <v>0.13715256897995801</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -7942,7 +7936,7 @@
         <v>0.274053880387848</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -7971,7 +7965,7 @@
         <v>0.324775909301532</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -8000,7 +7994,7 @@
         <v>0.24868421052631501</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -8029,7 +8023,7 @@
         <v>0.248073422655502</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -8058,7 +8052,7 @@
         <v>0.26561493234702799</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -8087,7 +8081,7 @@
         <v>0.13715256897995801</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -8116,7 +8110,7 @@
         <v>0.19559457364318</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -8145,7 +8139,7 @@
         <v>0.20469629267005099</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -8174,7 +8168,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -8203,7 +8197,7 @@
         <v>0.19934210526315699</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -8232,7 +8226,7 @@
         <v>0.103815789473684</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -8261,7 +8255,7 @@
         <v>6.6644736842105201E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -8290,7 +8284,7 @@
         <v>0.123328895154553</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -8319,7 +8313,7 @@
         <v>0.29188482445147901</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -8348,7 +8342,7 @@
         <v>0.36307771896847302</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -8377,7 +8371,7 @@
         <v>0.19934210526315699</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -8406,7 +8400,7 @@
         <v>0.244547326615594</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -8435,7 +8429,7 @@
         <v>0.27071162393861398</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -8464,7 +8458,7 @@
         <v>0.123328895154553</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -8493,7 +8487,7 @@
         <v>0.19421831740352299</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -8522,7 +8516,7 @@
         <v>0.20657291727735499</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1</v>
       </c>
@@ -8551,7 +8545,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -8580,7 +8574,7 @@
         <v>7.1710526315789405E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>3</v>
       </c>
@@ -8609,7 +8603,7 @@
         <v>3.6447368421052603E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -8638,7 +8632,7 @@
         <v>2.60526315789473E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -8667,7 +8661,7 @@
         <v>3.9450971177944799E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -8696,7 +8690,7 @@
         <v>9.7143330565248806E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -8725,7 +8719,7 @@
         <v>0.14074735263966501</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -8754,7 +8748,7 @@
         <v>7.1710526315789405E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -8783,7 +8777,7 @@
         <v>8.1361926240573895E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -8812,7 +8806,7 @@
         <v>9.7132169677947702E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>14</v>
       </c>
@@ -8841,7 +8835,7 @@
         <v>3.9450971177944799E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -8870,7 +8864,7 @@
         <v>6.13763537507045E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>16</v>
       </c>
@@ -8899,7 +8893,7 @@
         <v>6.8092234330894202E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>1</v>
       </c>
@@ -8928,7 +8922,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>2</v>
       </c>
@@ -8957,7 +8951,7 @@
         <v>1.3157894736842001E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>3</v>
       </c>
@@ -8986,7 +8980,7 @@
         <v>1.4605263157894699E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>4</v>
       </c>
@@ -9015,7 +9009,7 @@
         <v>1.8881578947368399E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -9044,7 +9038,7 @@
         <v>1.012145748987E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>7</v>
       </c>
@@ -9073,7 +9067,7 @@
         <v>3.5479919434212998E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>8</v>
       </c>
@@ -9102,7 +9096,7 @@
         <v>8.7976462115139306E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>10</v>
       </c>
@@ -9131,7 +9125,7 @@
         <v>1.3157894736842001E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>11</v>
       </c>
@@ -9160,7 +9154,7 @@
         <v>1.9739058548339801E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>12</v>
       </c>
@@ -9189,7 +9183,7 @@
         <v>4.0207449662581898E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -9218,7 +9212,7 @@
         <v>1.012145748987E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>15</v>
       </c>
@@ -9247,7 +9241,7 @@
         <v>9.1839847594695004E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>16</v>
       </c>
@@ -9276,7 +9270,7 @@
         <v>1.6739757807377499E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>1</v>
       </c>
@@ -9305,7 +9299,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>2</v>
       </c>
@@ -9397,7 +9391,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>3</v>
       </c>
@@ -9489,7 +9483,7 @@
         <v>0.87433628318584078</v>
       </c>
     </row>
-    <row r="74" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>4</v>
       </c>
@@ -9581,7 +9575,7 @@
         <v>0.86460176991150439</v>
       </c>
     </row>
-    <row r="75" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>6</v>
       </c>
@@ -9673,7 +9667,7 @@
         <v>0.86637168141592924</v>
       </c>
     </row>
-    <row r="76" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>7</v>
       </c>
@@ -9765,7 +9759,7 @@
         <v>0.86283185840707977</v>
       </c>
     </row>
-    <row r="77" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>8</v>
       </c>
@@ -9857,7 +9851,7 @@
         <v>0.87079646017699108</v>
       </c>
     </row>
-    <row r="78" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>10</v>
       </c>
@@ -9949,7 +9943,7 @@
         <v>0.86548672566371676</v>
       </c>
     </row>
-    <row r="79" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>11</v>
       </c>
@@ -10041,7 +10035,7 @@
         <v>0.86548672566371676</v>
       </c>
     </row>
-    <row r="80" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>12</v>
       </c>
@@ -10133,7 +10127,7 @@
         <v>0.86017699115044244</v>
       </c>
     </row>
-    <row r="81" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -10162,7 +10156,7 @@
         <v>3.4626038781163397E-5</v>
       </c>
     </row>
-    <row r="82" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>15</v>
       </c>
@@ -10191,7 +10185,7 @@
         <v>8.8079986149584404E-5</v>
       </c>
     </row>
-    <row r="83" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>16</v>
       </c>
@@ -10220,7 +10214,7 @@
         <v>8.8079986149584404E-5</v>
       </c>
     </row>
-    <row r="87" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>1</v>
       </c>
@@ -10312,300 +10306,300 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>2</v>
       </c>
       <c r="B88">
-        <v>0.62920353982300892</v>
+        <v>0.34424778761061942</v>
       </c>
       <c r="C88">
-        <v>0.62300884955752212</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="D88">
-        <v>0.62743362831858396</v>
+        <v>0.62566371681415922</v>
       </c>
       <c r="E88">
-        <v>0.61946902654867253</v>
+        <v>0.61592920353982294</v>
       </c>
       <c r="F88">
-        <v>0.61946902654867253</v>
+        <v>0.61327433628318573</v>
       </c>
       <c r="G88">
-        <v>0.62035398230088501</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="H88">
-        <v>0.63274336283185839</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="I88">
-        <v>0.62300884955752212</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="L88" t="s">
         <v>99</v>
       </c>
       <c r="M88">
-        <v>0.62920353982300892</v>
+        <v>0.34424778761061942</v>
       </c>
       <c r="N88">
-        <v>0.16814159292035391</v>
+        <v>0.1095575221238935</v>
       </c>
       <c r="O88">
-        <v>8.5132743362831803E-2</v>
+        <v>6.4513274336282997E-2</v>
       </c>
       <c r="P88">
-        <v>8.7433628318583992E-3</v>
+        <v>8.4424778761062001E-3</v>
       </c>
       <c r="Q88">
-        <v>0.62920353982300892</v>
+        <v>0.34424778761061942</v>
       </c>
       <c r="R88">
-        <v>0.84070796460176989</v>
+        <v>0.54778761061946901</v>
       </c>
       <c r="S88">
-        <v>0.85132743362831853</v>
+        <v>0.64513274336283177</v>
       </c>
       <c r="T88">
-        <v>0.87433628318584078</v>
+        <v>0.84424778761061936</v>
       </c>
       <c r="U88">
-        <v>0.62920353982300892</v>
+        <v>0.34424778761061942</v>
       </c>
       <c r="V88">
-        <v>0.75223240980849693</v>
+        <v>0.45191435477082248</v>
       </c>
       <c r="W88">
-        <v>0.75565007805945172</v>
+        <v>0.4834295304997836</v>
       </c>
       <c r="X88">
-        <v>0.76030110285253905</v>
+        <v>0.52517248409274941</v>
       </c>
       <c r="Y88">
-        <v>0.62920353982300892</v>
+        <v>0.34424778761061942</v>
       </c>
       <c r="Z88">
-        <v>0.72185840707964599</v>
+        <v>0.42007374631268429</v>
       </c>
       <c r="AA88">
-        <v>0.72325677763730856</v>
+        <v>0.43310226155358889</v>
       </c>
       <c r="AB88">
-        <v>0.72413532427085325</v>
+        <v>0.44137392430668798</v>
       </c>
       <c r="AC88">
-        <v>0.62920353982300892</v>
+        <v>0.34424778761061942</v>
       </c>
       <c r="AD88">
-        <v>0.84070796460176989</v>
+        <v>0.54778761061946901</v>
       </c>
       <c r="AE88">
-        <v>0.85132743362831853</v>
+        <v>0.64513274336283177</v>
       </c>
       <c r="AF88">
-        <v>0.87433628318584078</v>
-      </c>
-    </row>
-    <row r="89" spans="1:32" x14ac:dyDescent="0.2">
+        <v>0.84424778761061936</v>
+      </c>
+    </row>
+    <row r="89" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>3</v>
       </c>
       <c r="B89">
-        <v>0.16814159292035391</v>
+        <v>0.1095575221238935</v>
       </c>
       <c r="C89">
-        <v>0.16495575221238931</v>
+        <v>0.1653097345132743</v>
       </c>
       <c r="D89">
-        <v>0.16707964601769909</v>
+        <v>0.1672566371681416</v>
       </c>
       <c r="E89">
-        <v>0.1656637168141592</v>
+        <v>0.16548672566371669</v>
       </c>
       <c r="F89">
-        <v>0.16424778761061939</v>
+        <v>0.16318584070796449</v>
       </c>
       <c r="G89">
         <v>0.16495575221238931</v>
       </c>
       <c r="H89">
-        <v>0.16690265486725661</v>
+        <v>0.16707964601769909</v>
       </c>
       <c r="I89">
-        <v>0.16353982300884939</v>
+        <v>0.1647787610619468</v>
       </c>
       <c r="L89" t="s">
         <v>100</v>
       </c>
       <c r="M89">
-        <v>0.62300884955752212</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="N89">
-        <v>0.16495575221238931</v>
+        <v>0.1653097345132743</v>
       </c>
       <c r="O89">
-        <v>8.3716814159291997E-2</v>
+        <v>8.3893805309734504E-2</v>
       </c>
       <c r="P89">
-        <v>8.6460176991149992E-3</v>
+        <v>8.6814159292035002E-3</v>
       </c>
       <c r="Q89">
-        <v>0.62300884955752212</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="R89">
-        <v>0.82477876106194681</v>
+        <v>0.82654867256637166</v>
       </c>
       <c r="S89">
-        <v>0.8371681415929203</v>
+        <v>0.83893805309734515</v>
       </c>
       <c r="T89">
-        <v>0.86460176991150439</v>
+        <v>0.86814159292035398</v>
       </c>
       <c r="U89">
-        <v>0.62300884955752212</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="V89">
-        <v>0.7415343956944036</v>
+        <v>0.74167904013767016</v>
       </c>
       <c r="W89">
-        <v>0.7458116242261299</v>
+        <v>0.74570371874480279</v>
       </c>
       <c r="X89">
-        <v>0.75128517689708219</v>
+        <v>0.75113363554325607</v>
       </c>
       <c r="Y89">
-        <v>0.62300884955752212</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="Z89">
-        <v>0.71280235988200591</v>
+        <v>0.71246312684365765</v>
       </c>
       <c r="AA89">
-        <v>0.71472924568057306</v>
+        <v>0.71413681696867537</v>
       </c>
       <c r="AB89">
-        <v>0.71570067085624189</v>
+        <v>0.71493795019210093</v>
       </c>
       <c r="AC89">
-        <v>0.62300884955752212</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="AD89">
-        <v>0.82477876106194681</v>
+        <v>0.82654867256637166</v>
       </c>
       <c r="AE89">
-        <v>0.8371681415929203</v>
+        <v>0.83893805309734515</v>
       </c>
       <c r="AF89">
-        <v>0.86460176991150439</v>
-      </c>
-    </row>
-    <row r="90" spans="1:32" x14ac:dyDescent="0.2">
+        <v>0.86814159292035398</v>
+      </c>
+    </row>
+    <row r="90" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>4</v>
       </c>
       <c r="B90">
-        <v>8.5132743362831803E-2</v>
+        <v>6.4513274336282997E-2</v>
       </c>
       <c r="C90">
-        <v>8.3716814159291997E-2</v>
+        <v>8.3893805309734504E-2</v>
       </c>
       <c r="D90">
-        <v>8.4867256637168098E-2</v>
+        <v>8.44247787610619E-2</v>
       </c>
       <c r="E90">
-        <v>8.3893805309734504E-2</v>
+        <v>8.3628318584070799E-2</v>
       </c>
       <c r="F90">
-        <v>8.3628318584070799E-2</v>
+        <v>8.3539823008849504E-2</v>
       </c>
       <c r="G90">
-        <v>8.3716814159291997E-2</v>
+        <v>8.3805309734513195E-2</v>
       </c>
       <c r="H90">
-        <v>8.4513274336283098E-2</v>
+        <v>8.4690265486725605E-2</v>
       </c>
       <c r="I90">
-        <v>8.3097345132743305E-2</v>
+        <v>8.3362831858406997E-2</v>
       </c>
       <c r="L90" t="s">
         <v>101</v>
       </c>
       <c r="M90">
-        <v>0.62743362831858396</v>
+        <v>0.62566371681415922</v>
       </c>
       <c r="N90">
-        <v>0.16707964601769909</v>
+        <v>0.1672566371681416</v>
       </c>
       <c r="O90">
-        <v>8.4867256637168098E-2</v>
+        <v>8.44247787610619E-2</v>
       </c>
       <c r="P90">
-        <v>8.6637168141592003E-3</v>
+        <v>8.6460176991149992E-3</v>
       </c>
       <c r="Q90">
-        <v>0.62743362831858396</v>
+        <v>0.62566371681415922</v>
       </c>
       <c r="R90">
-        <v>0.83539823008849545</v>
+        <v>0.83628318584070782</v>
       </c>
       <c r="S90">
-        <v>0.84867256637168142</v>
+        <v>0.84424778761061958</v>
       </c>
       <c r="T90">
-        <v>0.86637168141592924</v>
+        <v>0.86460176991150439</v>
       </c>
       <c r="U90">
-        <v>0.62743362831858396</v>
+        <v>0.62566371681415922</v>
       </c>
       <c r="V90">
-        <v>0.74921276764635736</v>
+        <v>0.74872040639660964</v>
       </c>
       <c r="W90">
-        <v>0.75361302681350373</v>
+        <v>0.75129300719245173</v>
       </c>
       <c r="X90">
-        <v>0.75724205476213735</v>
+        <v>0.75569324226199253</v>
       </c>
       <c r="Y90">
-        <v>0.62743362831858396</v>
+        <v>0.62566371681415922</v>
       </c>
       <c r="Z90">
-        <v>0.71952802359881995</v>
+        <v>0.71861356932153397</v>
       </c>
       <c r="AA90">
-        <v>0.72140679870768365</v>
+        <v>0.71967376035960107</v>
       </c>
       <c r="AB90">
-        <v>0.72209482924078139</v>
+        <v>0.72059889693637558</v>
       </c>
       <c r="AC90">
-        <v>0.62743362831858396</v>
+        <v>0.62566371681415922</v>
       </c>
       <c r="AD90">
-        <v>0.83539823008849545</v>
+        <v>0.83628318584070782</v>
       </c>
       <c r="AE90">
-        <v>0.84867256637168142</v>
+        <v>0.84424778761061958</v>
       </c>
       <c r="AF90">
-        <v>0.86637168141592924</v>
-      </c>
-    </row>
-    <row r="91" spans="1:32" x14ac:dyDescent="0.2">
+        <v>0.86460176991150439</v>
+      </c>
+    </row>
+    <row r="91" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>5</v>
       </c>
       <c r="B91">
-        <v>8.7433628318583992E-3</v>
+        <v>8.4424778761062001E-3</v>
       </c>
       <c r="C91">
+        <v>8.6814159292035002E-3</v>
+      </c>
+      <c r="D91">
         <v>8.6460176991149992E-3</v>
       </c>
-      <c r="D91">
-        <v>8.6637168141592003E-3</v>
-      </c>
       <c r="E91">
-        <v>8.6283185840707998E-3</v>
+        <v>8.6371681415928995E-3</v>
       </c>
       <c r="F91">
-        <v>8.7079646017698999E-3</v>
+        <v>8.6725663716814005E-3</v>
       </c>
       <c r="G91">
         <v>8.6548672566371006E-3</v>
@@ -10614,366 +10608,366 @@
         <v>8.6548672566371006E-3</v>
       </c>
       <c r="I91">
-        <v>8.6017699115044002E-3</v>
+        <v>8.6460176991149992E-3</v>
       </c>
       <c r="L91" t="s">
         <v>102</v>
       </c>
       <c r="M91">
-        <v>0.61946902654867253</v>
+        <v>0.61592920353982294</v>
       </c>
       <c r="N91">
-        <v>0.1656637168141592</v>
+        <v>0.16548672566371669</v>
       </c>
       <c r="O91">
-        <v>8.3893805309734504E-2</v>
+        <v>8.3628318584070799E-2</v>
       </c>
       <c r="P91">
-        <v>8.6283185840707998E-3</v>
+        <v>8.6371681415928995E-3</v>
       </c>
       <c r="Q91">
-        <v>0.61946902654867253</v>
+        <v>0.61592920353982294</v>
       </c>
       <c r="R91">
-        <v>0.82831858407079628</v>
+        <v>0.82743362831858391</v>
       </c>
       <c r="S91">
-        <v>0.83893805309734515</v>
+        <v>0.83628318584070782</v>
       </c>
       <c r="T91">
-        <v>0.86283185840707977</v>
+        <v>0.86371681415929191</v>
       </c>
       <c r="U91">
-        <v>0.61946902654867253</v>
+        <v>0.61592920353982294</v>
       </c>
       <c r="V91">
-        <v>0.74143207160270697</v>
+        <v>0.73992854309119571</v>
       </c>
       <c r="W91">
-        <v>0.74491872960937111</v>
+        <v>0.7429352075230452</v>
       </c>
       <c r="X91">
-        <v>0.74978408834054755</v>
+        <v>0.74839396494972288</v>
       </c>
       <c r="Y91">
-        <v>0.61946902654867253</v>
+        <v>0.61592920353982294</v>
       </c>
       <c r="Z91">
-        <v>0.71154867256637166</v>
+        <v>0.70977876106194693</v>
       </c>
       <c r="AA91">
-        <v>0.71301973591796597</v>
+        <v>0.71110443882567775</v>
       </c>
       <c r="AB91">
-        <v>0.71394505844708278</v>
+        <v>0.7120941084865916</v>
       </c>
       <c r="AC91">
-        <v>0.61946902654867253</v>
+        <v>0.61592920353982294</v>
       </c>
       <c r="AD91">
-        <v>0.82831858407079628</v>
+        <v>0.82743362831858391</v>
       </c>
       <c r="AE91">
-        <v>0.83893805309734515</v>
+        <v>0.83628318584070782</v>
       </c>
       <c r="AF91">
-        <v>0.86283185840707977</v>
-      </c>
-    </row>
-    <row r="92" spans="1:32" x14ac:dyDescent="0.2">
+        <v>0.86371681415929191</v>
+      </c>
+    </row>
+    <row r="92" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>6</v>
       </c>
       <c r="B92">
-        <v>0.62920353982300892</v>
+        <v>0.34424778761061942</v>
       </c>
       <c r="C92">
-        <v>0.62300884955752212</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="D92">
-        <v>0.62743362831858396</v>
+        <v>0.62566371681415922</v>
       </c>
       <c r="E92">
-        <v>0.61946902654867253</v>
+        <v>0.61592920353982294</v>
       </c>
       <c r="F92">
-        <v>0.61946902654867253</v>
+        <v>0.61327433628318573</v>
       </c>
       <c r="G92">
-        <v>0.62035398230088501</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="H92">
-        <v>0.63274336283185839</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="I92">
-        <v>0.62300884955752212</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="L92" t="s">
         <v>103</v>
       </c>
       <c r="M92">
-        <v>0.61946902654867253</v>
+        <v>0.61327433628318573</v>
       </c>
       <c r="N92">
-        <v>0.16424778761061939</v>
+        <v>0.16318584070796449</v>
       </c>
       <c r="O92">
-        <v>8.3628318584070799E-2</v>
+        <v>8.3539823008849504E-2</v>
       </c>
       <c r="P92">
-        <v>8.7079646017698999E-3</v>
+        <v>8.6725663716814005E-3</v>
       </c>
       <c r="Q92">
-        <v>0.61946902654867253</v>
+        <v>0.61327433628318573</v>
       </c>
       <c r="R92">
-        <v>0.82123893805309733</v>
+        <v>0.81592920353982312</v>
       </c>
       <c r="S92">
-        <v>0.83628318584070804</v>
+        <v>0.83539823008849567</v>
       </c>
       <c r="T92">
-        <v>0.87079646017699108</v>
+        <v>0.86725663716814161</v>
       </c>
       <c r="U92">
-        <v>0.61946902654867253</v>
+        <v>0.61327433628318573</v>
       </c>
       <c r="V92">
-        <v>0.73728826916094825</v>
+        <v>0.73212857139942233</v>
       </c>
       <c r="W92">
-        <v>0.74232327273207699</v>
+        <v>0.73842433237667227</v>
       </c>
       <c r="X92">
-        <v>0.74946048218436134</v>
+        <v>0.74470896382332741</v>
       </c>
       <c r="Y92">
-        <v>0.61946902654867253</v>
+        <v>0.61327433628318573</v>
       </c>
       <c r="Z92">
-        <v>0.70839233038348071</v>
+        <v>0.70324483775811208</v>
       </c>
       <c r="AA92">
-        <v>0.7105734653743504</v>
+        <v>0.70584211265627195</v>
       </c>
       <c r="AB92">
-        <v>0.71195529433083737</v>
+        <v>0.70689506514116796</v>
       </c>
       <c r="AC92">
-        <v>0.61946902654867253</v>
+        <v>0.61327433628318573</v>
       </c>
       <c r="AD92">
-        <v>0.82123893805309733</v>
+        <v>0.81592920353982312</v>
       </c>
       <c r="AE92">
-        <v>0.83628318584070804</v>
+        <v>0.83539823008849567</v>
       </c>
       <c r="AF92">
-        <v>0.87079646017699108</v>
-      </c>
-    </row>
-    <row r="93" spans="1:32" x14ac:dyDescent="0.2">
+        <v>0.86725663716814161</v>
+      </c>
+    </row>
+    <row r="93" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>7</v>
       </c>
       <c r="B93">
-        <v>0.84070796460176989</v>
+        <v>0.54778761061946901</v>
       </c>
       <c r="C93">
-        <v>0.82477876106194681</v>
+        <v>0.82654867256637166</v>
       </c>
       <c r="D93">
-        <v>0.83539823008849545</v>
+        <v>0.83628318584070782</v>
       </c>
       <c r="E93">
-        <v>0.82831858407079628</v>
+        <v>0.82743362831858391</v>
       </c>
       <c r="F93">
-        <v>0.82123893805309733</v>
+        <v>0.81592920353982312</v>
       </c>
       <c r="G93">
         <v>0.82477876106194681</v>
       </c>
       <c r="H93">
-        <v>0.8345132743362832</v>
+        <v>0.83539823008849567</v>
       </c>
       <c r="I93">
-        <v>0.81769911504424775</v>
+        <v>0.82389380530973444</v>
       </c>
       <c r="L93" t="s">
         <v>104</v>
       </c>
       <c r="M93">
-        <v>0.62035398230088501</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="N93">
         <v>0.16495575221238931</v>
       </c>
       <c r="O93">
-        <v>8.3716814159291997E-2</v>
+        <v>8.3805309734513195E-2</v>
       </c>
       <c r="P93">
         <v>8.6548672566371006E-3</v>
       </c>
       <c r="Q93">
-        <v>0.62035398230088501</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="R93">
         <v>0.82477876106194681</v>
       </c>
       <c r="S93">
-        <v>0.8371681415929203</v>
+        <v>0.83805309734513267</v>
       </c>
       <c r="T93">
         <v>0.86548672566371676</v>
       </c>
       <c r="U93">
-        <v>0.62035398230088501</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="V93">
-        <v>0.73909805936333373</v>
+        <v>0.73948967234156338</v>
       </c>
       <c r="W93">
-        <v>0.74321829309646603</v>
+        <v>0.74378386970299437</v>
       </c>
       <c r="X93">
-        <v>0.74882371759365562</v>
+        <v>0.7492237815007089</v>
       </c>
       <c r="Y93">
-        <v>0.62035398230088501</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="Z93">
-        <v>0.70966076696165181</v>
+        <v>0.71023598820058997</v>
       </c>
       <c r="AA93">
-        <v>0.71142786908273625</v>
+        <v>0.71200906026127275</v>
       </c>
       <c r="AB93">
-        <v>0.71240030930980858</v>
+        <v>0.71298017721829265</v>
       </c>
       <c r="AC93">
-        <v>0.62035398230088501</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="AD93">
         <v>0.82477876106194681</v>
       </c>
       <c r="AE93">
-        <v>0.8371681415929203</v>
+        <v>0.83805309734513267</v>
       </c>
       <c r="AF93">
         <v>0.86548672566371676</v>
       </c>
     </row>
-    <row r="94" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>8</v>
       </c>
       <c r="B94">
-        <v>0.85132743362831853</v>
+        <v>0.64513274336283177</v>
       </c>
       <c r="C94">
-        <v>0.8371681415929203</v>
+        <v>0.83893805309734515</v>
       </c>
       <c r="D94">
-        <v>0.84867256637168142</v>
+        <v>0.84424778761061958</v>
       </c>
       <c r="E94">
-        <v>0.83893805309734515</v>
+        <v>0.83628318584070782</v>
       </c>
       <c r="F94">
-        <v>0.83628318584070804</v>
+        <v>0.83539823008849567</v>
       </c>
       <c r="G94">
-        <v>0.8371681415929203</v>
+        <v>0.83805309734513267</v>
       </c>
       <c r="H94">
-        <v>0.84513274336283184</v>
+        <v>0.84690265486725669</v>
       </c>
       <c r="I94">
-        <v>0.83097345132743372</v>
+        <v>0.83362831858407083</v>
       </c>
       <c r="L94" t="s">
         <v>105</v>
       </c>
       <c r="M94">
-        <v>0.63274336283185839</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="N94">
-        <v>0.16690265486725661</v>
+        <v>0.16707964601769909</v>
       </c>
       <c r="O94">
-        <v>8.4513274336283098E-2</v>
+        <v>8.4690265486725605E-2</v>
       </c>
       <c r="P94">
         <v>8.6548672566371006E-3</v>
       </c>
       <c r="Q94">
-        <v>0.63274336283185839</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="R94">
-        <v>0.8345132743362832</v>
+        <v>0.83539823008849567</v>
       </c>
       <c r="S94">
-        <v>0.84513274336283184</v>
+        <v>0.84690265486725669</v>
       </c>
       <c r="T94">
         <v>0.86548672566371676</v>
       </c>
       <c r="U94">
-        <v>0.63274336283185839</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="V94">
-        <v>0.75075982941528285</v>
+        <v>0.7500509685462633</v>
       </c>
       <c r="W94">
-        <v>0.75441276183895867</v>
+        <v>0.75385285415213787</v>
       </c>
       <c r="X94">
-        <v>0.75850986732845715</v>
+        <v>0.75731407461203493</v>
       </c>
       <c r="Y94">
-        <v>0.63274336283185839</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="Z94">
-        <v>0.72190265486725658</v>
+        <v>0.72072271386430675</v>
       </c>
       <c r="AA94">
-        <v>0.7235391206630144</v>
+        <v>0.72234126984126967</v>
       </c>
       <c r="AB94">
-        <v>0.72425221734611522</v>
+        <v>0.72285130294618338</v>
       </c>
       <c r="AC94">
-        <v>0.63274336283185839</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="AD94">
-        <v>0.8345132743362832</v>
+        <v>0.83539823008849567</v>
       </c>
       <c r="AE94">
-        <v>0.84513274336283184</v>
+        <v>0.84690265486725669</v>
       </c>
       <c r="AF94">
         <v>0.86548672566371676</v>
       </c>
     </row>
-    <row r="95" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>9</v>
       </c>
       <c r="B95">
-        <v>0.87433628318584078</v>
+        <v>0.84424778761061936</v>
       </c>
       <c r="C95">
+        <v>0.86814159292035398</v>
+      </c>
+      <c r="D95">
         <v>0.86460176991150439</v>
       </c>
-      <c r="D95">
-        <v>0.86637168141592924</v>
-      </c>
       <c r="E95">
-        <v>0.86283185840707977</v>
+        <v>0.86371681415929191</v>
       </c>
       <c r="F95">
-        <v>0.87079646017699108</v>
+        <v>0.86725663716814161</v>
       </c>
       <c r="G95">
         <v>0.86548672566371676</v>
@@ -10982,409 +10976,409 @@
         <v>0.86548672566371676</v>
       </c>
       <c r="I95">
-        <v>0.86017699115044244</v>
+        <v>0.8646017699115045</v>
       </c>
       <c r="L95" t="s">
         <v>106</v>
       </c>
       <c r="M95">
-        <v>0.62300884955752212</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="N95">
-        <v>0.16353982300884939</v>
+        <v>0.1647787610619468</v>
       </c>
       <c r="O95">
-        <v>8.3097345132743305E-2</v>
+        <v>8.3362831858406997E-2</v>
       </c>
       <c r="P95">
-        <v>8.6017699115044002E-3</v>
+        <v>8.6460176991149992E-3</v>
       </c>
       <c r="Q95">
-        <v>0.62300884955752212</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="R95">
-        <v>0.81769911504424775</v>
+        <v>0.82389380530973444</v>
       </c>
       <c r="S95">
-        <v>0.83097345132743372</v>
+        <v>0.83362831858407083</v>
       </c>
       <c r="T95">
-        <v>0.86017699115044244</v>
+        <v>0.8646017699115045</v>
       </c>
       <c r="U95">
-        <v>0.62300884955752212</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="V95">
-        <v>0.73668125318101874</v>
+        <v>0.74347147090489041</v>
       </c>
       <c r="W95">
-        <v>0.74110394028228066</v>
+        <v>0.74684219230890991</v>
       </c>
       <c r="X95">
-        <v>0.74677607454431738</v>
+        <v>0.75271844974994939</v>
       </c>
       <c r="Y95">
-        <v>0.62300884955752212</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="Z95">
-        <v>0.70877581120943955</v>
+        <v>0.71584070796460164</v>
       </c>
       <c r="AA95">
-        <v>0.71067811490377863</v>
+        <v>0.71736304256215755</v>
       </c>
       <c r="AB95">
-        <v>0.71162156178649771</v>
+        <v>0.71827337168777072</v>
       </c>
       <c r="AC95">
-        <v>0.62300884955752212</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="AD95">
-        <v>0.81769911504424775</v>
+        <v>0.82389380530973444</v>
       </c>
       <c r="AE95">
-        <v>0.83097345132743372</v>
+        <v>0.83362831858407083</v>
       </c>
       <c r="AF95">
-        <v>0.86017699115044244</v>
-      </c>
-    </row>
-    <row r="96" spans="1:32" x14ac:dyDescent="0.2">
+        <v>0.8646017699115045</v>
+      </c>
+    </row>
+    <row r="96" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>10</v>
       </c>
       <c r="B96">
-        <v>0.62920353982300892</v>
+        <v>0.34424778761061942</v>
       </c>
       <c r="C96">
-        <v>0.62300884955752212</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="D96">
-        <v>0.62743362831858396</v>
+        <v>0.62566371681415922</v>
       </c>
       <c r="E96">
-        <v>0.61946902654867253</v>
+        <v>0.61592920353982294</v>
       </c>
       <c r="F96">
-        <v>0.61946902654867253</v>
+        <v>0.61327433628318573</v>
       </c>
       <c r="G96">
-        <v>0.62035398230088501</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="H96">
-        <v>0.63274336283185839</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="I96">
-        <v>0.62300884955752212</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.63185840707964602</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>11</v>
       </c>
       <c r="B97">
-        <v>0.75223240980849693</v>
+        <v>0.45191435477082248</v>
       </c>
       <c r="C97">
-        <v>0.7415343956944036</v>
+        <v>0.74167904013767016</v>
       </c>
       <c r="D97">
-        <v>0.74921276764635736</v>
+        <v>0.74872040639660964</v>
       </c>
       <c r="E97">
-        <v>0.74143207160270697</v>
+        <v>0.73992854309119571</v>
       </c>
       <c r="F97">
-        <v>0.73728826916094825</v>
+        <v>0.73212857139942233</v>
       </c>
       <c r="G97">
-        <v>0.73909805936333373</v>
+        <v>0.73948967234156338</v>
       </c>
       <c r="H97">
-        <v>0.75075982941528285</v>
+        <v>0.7500509685462633</v>
       </c>
       <c r="I97">
-        <v>0.73668125318101874</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.74347147090489041</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>12</v>
       </c>
       <c r="B98">
-        <v>0.75565007805945172</v>
+        <v>0.4834295304997836</v>
       </c>
       <c r="C98">
-        <v>0.7458116242261299</v>
+        <v>0.74570371874480279</v>
       </c>
       <c r="D98">
-        <v>0.75361302681350373</v>
+        <v>0.75129300719245173</v>
       </c>
       <c r="E98">
-        <v>0.74491872960937111</v>
+        <v>0.7429352075230452</v>
       </c>
       <c r="F98">
-        <v>0.74232327273207699</v>
+        <v>0.73842433237667227</v>
       </c>
       <c r="G98">
-        <v>0.74321829309646603</v>
+        <v>0.74378386970299437</v>
       </c>
       <c r="H98">
-        <v>0.75441276183895867</v>
+        <v>0.75385285415213787</v>
       </c>
       <c r="I98">
-        <v>0.74110394028228066</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.74684219230890991</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>13</v>
       </c>
       <c r="B99">
-        <v>0.76030110285253905</v>
+        <v>0.52517248409274941</v>
       </c>
       <c r="C99">
-        <v>0.75128517689708219</v>
+        <v>0.75113363554325607</v>
       </c>
       <c r="D99">
-        <v>0.75724205476213735</v>
+        <v>0.75569324226199253</v>
       </c>
       <c r="E99">
-        <v>0.74978408834054755</v>
+        <v>0.74839396494972288</v>
       </c>
       <c r="F99">
-        <v>0.74946048218436134</v>
+        <v>0.74470896382332741</v>
       </c>
       <c r="G99">
-        <v>0.74882371759365562</v>
+        <v>0.7492237815007089</v>
       </c>
       <c r="H99">
-        <v>0.75850986732845715</v>
+        <v>0.75731407461203493</v>
       </c>
       <c r="I99">
-        <v>0.74677607454431738</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.75271844974994939</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>14</v>
       </c>
       <c r="B100">
-        <v>0.62920353982300892</v>
+        <v>0.34424778761061942</v>
       </c>
       <c r="C100">
-        <v>0.62300884955752212</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="D100">
-        <v>0.62743362831858396</v>
+        <v>0.62566371681415922</v>
       </c>
       <c r="E100">
-        <v>0.61946902654867253</v>
+        <v>0.61592920353982294</v>
       </c>
       <c r="F100">
-        <v>0.61946902654867253</v>
+        <v>0.61327433628318573</v>
       </c>
       <c r="G100">
-        <v>0.62035398230088501</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="H100">
-        <v>0.63274336283185839</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="I100">
-        <v>0.62300884955752212</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.63185840707964602</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>15</v>
       </c>
       <c r="B101">
-        <v>0.72185840707964599</v>
+        <v>0.42007374631268429</v>
       </c>
       <c r="C101">
-        <v>0.71280235988200591</v>
+        <v>0.71246312684365765</v>
       </c>
       <c r="D101">
-        <v>0.71952802359881995</v>
+        <v>0.71861356932153397</v>
       </c>
       <c r="E101">
-        <v>0.71154867256637166</v>
+        <v>0.70977876106194693</v>
       </c>
       <c r="F101">
-        <v>0.70839233038348071</v>
+        <v>0.70324483775811208</v>
       </c>
       <c r="G101">
-        <v>0.70966076696165181</v>
+        <v>0.71023598820058997</v>
       </c>
       <c r="H101">
-        <v>0.72190265486725658</v>
+        <v>0.72072271386430675</v>
       </c>
       <c r="I101">
-        <v>0.70877581120943955</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.71584070796460164</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>16</v>
       </c>
       <c r="B102">
-        <v>0.72325677763730856</v>
+        <v>0.43310226155358889</v>
       </c>
       <c r="C102">
-        <v>0.71472924568057306</v>
+        <v>0.71413681696867537</v>
       </c>
       <c r="D102">
-        <v>0.72140679870768365</v>
+        <v>0.71967376035960107</v>
       </c>
       <c r="E102">
-        <v>0.71301973591796597</v>
+        <v>0.71110443882567775</v>
       </c>
       <c r="F102">
-        <v>0.7105734653743504</v>
+        <v>0.70584211265627195</v>
       </c>
       <c r="G102">
-        <v>0.71142786908273625</v>
+        <v>0.71200906026127275</v>
       </c>
       <c r="H102">
-        <v>0.7235391206630144</v>
+        <v>0.72234126984126967</v>
       </c>
       <c r="I102">
-        <v>0.71067811490377863</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.71736304256215755</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>17</v>
       </c>
       <c r="B103">
-        <v>0.72413532427085325</v>
+        <v>0.44137392430668798</v>
       </c>
       <c r="C103">
-        <v>0.71570067085624189</v>
+        <v>0.71493795019210093</v>
       </c>
       <c r="D103">
-        <v>0.72209482924078139</v>
+        <v>0.72059889693637558</v>
       </c>
       <c r="E103">
-        <v>0.71394505844708278</v>
+        <v>0.7120941084865916</v>
       </c>
       <c r="F103">
-        <v>0.71195529433083737</v>
+        <v>0.70689506514116796</v>
       </c>
       <c r="G103">
-        <v>0.71240030930980858</v>
+        <v>0.71298017721829265</v>
       </c>
       <c r="H103">
-        <v>0.72425221734611522</v>
+        <v>0.72285130294618338</v>
       </c>
       <c r="I103">
-        <v>0.71162156178649771</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.71827337168777072</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>18</v>
       </c>
       <c r="B104">
-        <v>0.62920353982300892</v>
+        <v>0.34424778761061942</v>
       </c>
       <c r="C104">
-        <v>0.62300884955752212</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="D104">
-        <v>0.62743362831858396</v>
+        <v>0.62566371681415922</v>
       </c>
       <c r="E104">
-        <v>0.61946902654867253</v>
+        <v>0.61592920353982294</v>
       </c>
       <c r="F104">
-        <v>0.61946902654867253</v>
+        <v>0.61327433628318573</v>
       </c>
       <c r="G104">
-        <v>0.62035398230088501</v>
+        <v>0.62212389380530975</v>
       </c>
       <c r="H104">
-        <v>0.63274336283185839</v>
+        <v>0.63185840707964602</v>
       </c>
       <c r="I104">
-        <v>0.62300884955752212</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.63185840707964602</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>19</v>
       </c>
       <c r="B105">
-        <v>0.84070796460176989</v>
+        <v>0.54778761061946901</v>
       </c>
       <c r="C105">
-        <v>0.82477876106194681</v>
+        <v>0.82654867256637166</v>
       </c>
       <c r="D105">
-        <v>0.83539823008849545</v>
+        <v>0.83628318584070782</v>
       </c>
       <c r="E105">
-        <v>0.82831858407079628</v>
+        <v>0.82743362831858391</v>
       </c>
       <c r="F105">
-        <v>0.82123893805309733</v>
+        <v>0.81592920353982312</v>
       </c>
       <c r="G105">
         <v>0.82477876106194681</v>
       </c>
       <c r="H105">
-        <v>0.8345132743362832</v>
+        <v>0.83539823008849567</v>
       </c>
       <c r="I105">
-        <v>0.81769911504424775</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.82389380530973444</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>20</v>
       </c>
       <c r="B106">
-        <v>0.85132743362831853</v>
+        <v>0.64513274336283177</v>
       </c>
       <c r="C106">
-        <v>0.8371681415929203</v>
+        <v>0.83893805309734515</v>
       </c>
       <c r="D106">
-        <v>0.84867256637168142</v>
+        <v>0.84424778761061958</v>
       </c>
       <c r="E106">
-        <v>0.83893805309734515</v>
+        <v>0.83628318584070782</v>
       </c>
       <c r="F106">
-        <v>0.83628318584070804</v>
+        <v>0.83539823008849567</v>
       </c>
       <c r="G106">
-        <v>0.8371681415929203</v>
+        <v>0.83805309734513267</v>
       </c>
       <c r="H106">
-        <v>0.84513274336283184</v>
+        <v>0.84690265486725669</v>
       </c>
       <c r="I106">
-        <v>0.83097345132743372</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.83362831858407083</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>21</v>
       </c>
       <c r="B107">
-        <v>0.87433628318584078</v>
+        <v>0.84424778761061936</v>
       </c>
       <c r="C107">
+        <v>0.86814159292035398</v>
+      </c>
+      <c r="D107">
         <v>0.86460176991150439</v>
       </c>
-      <c r="D107">
-        <v>0.86637168141592924</v>
-      </c>
       <c r="E107">
-        <v>0.86283185840707977</v>
+        <v>0.86371681415929191</v>
       </c>
       <c r="F107">
-        <v>0.87079646017699108</v>
+        <v>0.86725663716814161</v>
       </c>
       <c r="G107">
         <v>0.86548672566371676</v>
@@ -11393,7 +11387,7 @@
         <v>0.86548672566371676</v>
       </c>
       <c r="I107">
-        <v>0.86017699115044244</v>
+        <v>0.8646017699115045</v>
       </c>
     </row>
   </sheetData>
@@ -11413,17 +11407,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBAEBD0B-6C2A-4EF8-8936-3C4C027D1B7C}">
   <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3:AB10"/>
+    <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z12" sqref="Z12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="25" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="25" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>84</v>
       </c>
@@ -11470,7 +11464,7 @@
       <c r="AB1" s="21"/>
       <c r="AC1" s="21"/>
     </row>
-    <row r="2" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23"/>
       <c r="B2" s="8" t="s">
         <v>87</v>
@@ -11557,7 +11551,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>76</v>
       </c>
@@ -11634,19 +11628,19 @@
         <v>4.3859649122807001E-5</v>
       </c>
       <c r="Z3" s="18">
-        <v>0.62920353982300892</v>
+        <v>0.34424778761061942</v>
       </c>
       <c r="AA3" s="13">
-        <v>0.84070796460176989</v>
+        <v>0.54778761061946901</v>
       </c>
       <c r="AB3" s="18">
-        <v>0.75223240980849693</v>
+        <v>0.45191435477082248</v>
       </c>
       <c r="AC3" s="13">
-        <v>0.72185840707964599</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+        <v>0.42007374631268429</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>77</v>
       </c>
@@ -11722,20 +11716,20 @@
       <c r="Y4" s="11">
         <v>1.49521531100478E-5</v>
       </c>
-      <c r="Z4" s="24">
-        <v>0.62035398230088501</v>
-      </c>
-      <c r="AA4" s="24">
+      <c r="Z4" s="11">
+        <v>0.62212389380530975</v>
+      </c>
+      <c r="AA4" s="11">
         <v>0.82477876106194681</v>
       </c>
-      <c r="AB4" s="24">
-        <v>0.73909805936333373</v>
-      </c>
-      <c r="AC4" s="24">
-        <v>0.70966076696165181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AB4" s="11">
+        <v>0.73948967234156338</v>
+      </c>
+      <c r="AC4" s="11">
+        <v>0.71023598820058997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>78</v>
       </c>
@@ -11811,20 +11805,20 @@
       <c r="Y5" s="15">
         <v>4.4956140350869999E-4</v>
       </c>
-      <c r="Z5" s="24">
-        <v>0.61946902654867253</v>
-      </c>
-      <c r="AA5" s="24">
-        <v>0.82123893805309733</v>
-      </c>
-      <c r="AB5" s="24">
-        <v>0.73728826916094825</v>
-      </c>
-      <c r="AC5" s="24">
-        <v>0.70839233038348071</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="Z5" s="11">
+        <v>0.61327433628318573</v>
+      </c>
+      <c r="AA5" s="11">
+        <v>0.81592920353982312</v>
+      </c>
+      <c r="AB5" s="11">
+        <v>0.73212857139942233</v>
+      </c>
+      <c r="AC5" s="11">
+        <v>0.70324483775811208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>79</v>
       </c>
@@ -11900,20 +11894,20 @@
       <c r="Y6" s="11">
         <v>3.2894736842099999E-4</v>
       </c>
-      <c r="Z6" s="24">
-        <v>0.62300884955752212</v>
-      </c>
-      <c r="AA6" s="24">
-        <v>0.82477876106194681</v>
-      </c>
-      <c r="AB6" s="24">
-        <v>0.7415343956944036</v>
-      </c>
-      <c r="AC6" s="24">
-        <v>0.71280235988200591</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="Z6" s="11">
+        <v>0.62212389380530975</v>
+      </c>
+      <c r="AA6" s="11">
+        <v>0.82654867256637166</v>
+      </c>
+      <c r="AB6" s="11">
+        <v>0.74167904013767016</v>
+      </c>
+      <c r="AC6" s="11">
+        <v>0.71246312684365765</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>80</v>
       </c>
@@ -11989,20 +11983,20 @@
       <c r="Y7" s="11">
         <v>0</v>
       </c>
-      <c r="Z7" s="24">
-        <v>0.61946902654867253</v>
-      </c>
-      <c r="AA7" s="24">
-        <v>0.82831858407079628</v>
-      </c>
-      <c r="AB7" s="24">
-        <v>0.74143207160270697</v>
-      </c>
-      <c r="AC7" s="24">
-        <v>0.71154867256637166</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="Z7" s="11">
+        <v>0.61592920353982294</v>
+      </c>
+      <c r="AA7" s="11">
+        <v>0.82743362831858391</v>
+      </c>
+      <c r="AB7" s="11">
+        <v>0.73992854309119571</v>
+      </c>
+      <c r="AC7" s="11">
+        <v>0.70977876106194693</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>81</v>
       </c>
@@ -12078,20 +12072,20 @@
       <c r="Y8" s="16">
         <v>1.2260765550239001E-3</v>
       </c>
-      <c r="Z8" s="24">
-        <v>0.62743362831858396</v>
+      <c r="Z8" s="11">
+        <v>0.62566371681415922</v>
       </c>
       <c r="AA8" s="15">
-        <v>0.83539823008849545</v>
-      </c>
-      <c r="AB8" s="24">
-        <v>0.74921276764635736</v>
+        <v>0.83628318584070782</v>
+      </c>
+      <c r="AB8" s="11">
+        <v>0.74872040639660964</v>
       </c>
       <c r="AC8" s="15">
-        <v>0.71952802359881995</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+        <v>0.71861356932153397</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>82</v>
       </c>
@@ -12168,19 +12162,19 @@
         <v>1.3157894736839999E-4</v>
       </c>
       <c r="Z9" s="16">
-        <v>0.63274336283185839</v>
-      </c>
-      <c r="AA9" s="24">
-        <v>0.8345132743362832</v>
+        <v>0.63185840707964602</v>
+      </c>
+      <c r="AA9" s="11">
+        <v>0.83539823008849567</v>
       </c>
       <c r="AB9" s="16">
-        <v>0.75075982941528285</v>
+        <v>0.7500509685462633</v>
       </c>
       <c r="AC9" s="16">
-        <v>0.72190265486725658</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+        <v>0.72072271386430675</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>83</v>
       </c>
@@ -12256,17 +12250,17 @@
       <c r="Y10" s="12">
         <v>8.8079986149584404E-5</v>
       </c>
-      <c r="Z10" s="25">
-        <v>0.62300884955752212</v>
-      </c>
-      <c r="AA10" s="25">
-        <v>0.81769911504424775</v>
-      </c>
-      <c r="AB10" s="25">
-        <v>0.73668125318101874</v>
-      </c>
-      <c r="AC10" s="25">
-        <v>0.70877581120943955</v>
+      <c r="Z10" s="12">
+        <v>0.63185840707964602</v>
+      </c>
+      <c r="AA10" s="12">
+        <v>0.82389380530973444</v>
+      </c>
+      <c r="AB10" s="12">
+        <v>0.74347147090489041</v>
+      </c>
+      <c r="AC10" s="12">
+        <v>0.71584070796460164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
charts for semeval14-rest for cat
</commit_message>
<xml_diff>
--- a/output/SemEval-14/Restaurants/agg.pred.eval.mean.20.0.0.xlsx
+++ b/output/SemEval-14/Restaurants/agg.pred.eval.mean.20.0.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farinam\PycharmProjects\LADy\output\SemEval-14\Restaurants\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Github\Fani-Lab\lady\main\output\SemEval-14\Restaurants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE9C910-FA39-4DE0-BC5F-D30F31493DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6875CC13-A205-4444-9B9F-A20CAFB7BCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{1230938A-22E1-464A-B275-4F8E3DAF70F5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{1230938A-22E1-464A-B275-4F8E3DAF70F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -543,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -612,11 +612,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -928,7 +1001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F85FE2-0E4A-4FDA-8B9D-4C7A407A54D4}">
   <dimension ref="A1:I153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+    <sheetView topLeftCell="A118" workbookViewId="0">
       <selection activeCell="A134" sqref="A134:I153"/>
     </sheetView>
   </sheetViews>
@@ -11407,8 +11480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBAEBD0B-6C2A-4EF8-8936-3C4C027D1B7C}">
   <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z12" sqref="Z12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11627,16 +11700,16 @@
       <c r="Y3" s="10">
         <v>4.3859649122807001E-5</v>
       </c>
-      <c r="Z3" s="18">
-        <v>0.34424778761061942</v>
-      </c>
-      <c r="AA3" s="13">
+      <c r="Z3" s="27">
+        <v>0.34424778761061903</v>
+      </c>
+      <c r="AA3" s="27">
         <v>0.54778761061946901</v>
       </c>
-      <c r="AB3" s="18">
+      <c r="AB3" s="27">
         <v>0.45191435477082248</v>
       </c>
-      <c r="AC3" s="13">
+      <c r="AC3" s="27">
         <v>0.42007374631268429</v>
       </c>
     </row>
@@ -11716,16 +11789,16 @@
       <c r="Y4" s="11">
         <v>1.49521531100478E-5</v>
       </c>
-      <c r="Z4" s="11">
+      <c r="Z4" s="28">
         <v>0.62212389380530975</v>
       </c>
-      <c r="AA4" s="11">
+      <c r="AA4" s="28">
         <v>0.82477876106194681</v>
       </c>
-      <c r="AB4" s="11">
+      <c r="AB4" s="28">
         <v>0.73948967234156338</v>
       </c>
-      <c r="AC4" s="11">
+      <c r="AC4" s="28">
         <v>0.71023598820058997</v>
       </c>
     </row>
@@ -11805,16 +11878,16 @@
       <c r="Y5" s="15">
         <v>4.4956140350869999E-4</v>
       </c>
-      <c r="Z5" s="11">
+      <c r="Z5" s="28">
         <v>0.61327433628318573</v>
       </c>
-      <c r="AA5" s="11">
+      <c r="AA5" s="28">
         <v>0.81592920353982312</v>
       </c>
-      <c r="AB5" s="11">
+      <c r="AB5" s="28">
         <v>0.73212857139942233</v>
       </c>
-      <c r="AC5" s="11">
+      <c r="AC5" s="28">
         <v>0.70324483775811208</v>
       </c>
     </row>
@@ -11894,16 +11967,16 @@
       <c r="Y6" s="11">
         <v>3.2894736842099999E-4</v>
       </c>
-      <c r="Z6" s="11">
+      <c r="Z6" s="28">
         <v>0.62212389380530975</v>
       </c>
-      <c r="AA6" s="11">
+      <c r="AA6" s="28">
         <v>0.82654867256637166</v>
       </c>
-      <c r="AB6" s="11">
+      <c r="AB6" s="28">
         <v>0.74167904013767016</v>
       </c>
-      <c r="AC6" s="11">
+      <c r="AC6" s="28">
         <v>0.71246312684365765</v>
       </c>
     </row>
@@ -11983,16 +12056,16 @@
       <c r="Y7" s="11">
         <v>0</v>
       </c>
-      <c r="Z7" s="11">
+      <c r="Z7" s="28">
         <v>0.61592920353982294</v>
       </c>
-      <c r="AA7" s="11">
+      <c r="AA7" s="28">
         <v>0.82743362831858391</v>
       </c>
-      <c r="AB7" s="11">
+      <c r="AB7" s="28">
         <v>0.73992854309119571</v>
       </c>
-      <c r="AC7" s="11">
+      <c r="AC7" s="28">
         <v>0.70977876106194693</v>
       </c>
     </row>
@@ -12072,16 +12145,16 @@
       <c r="Y8" s="16">
         <v>1.2260765550239001E-3</v>
       </c>
-      <c r="Z8" s="11">
+      <c r="Z8" s="24">
         <v>0.62566371681415922</v>
       </c>
-      <c r="AA8" s="15">
+      <c r="AA8" s="25">
         <v>0.83628318584070782</v>
       </c>
-      <c r="AB8" s="11">
+      <c r="AB8" s="24">
         <v>0.74872040639660964</v>
       </c>
-      <c r="AC8" s="15">
+      <c r="AC8" s="24">
         <v>0.71861356932153397</v>
       </c>
     </row>
@@ -12161,16 +12234,16 @@
       <c r="Y9" s="11">
         <v>1.3157894736839999E-4</v>
       </c>
-      <c r="Z9" s="16">
+      <c r="Z9" s="25">
         <v>0.63185840707964602</v>
       </c>
-      <c r="AA9" s="11">
+      <c r="AA9" s="24">
         <v>0.83539823008849567</v>
       </c>
-      <c r="AB9" s="16">
+      <c r="AB9" s="25">
         <v>0.7500509685462633</v>
       </c>
-      <c r="AC9" s="16">
+      <c r="AC9" s="25">
         <v>0.72072271386430675</v>
       </c>
     </row>
@@ -12250,16 +12323,16 @@
       <c r="Y10" s="12">
         <v>8.8079986149584404E-5</v>
       </c>
-      <c r="Z10" s="12">
+      <c r="Z10" s="26">
         <v>0.63185840707964602</v>
       </c>
-      <c r="AA10" s="12">
+      <c r="AA10" s="29">
         <v>0.82389380530973444</v>
       </c>
-      <c r="AB10" s="12">
+      <c r="AB10" s="29">
         <v>0.74347147090489041</v>
       </c>
-      <c r="AC10" s="12">
+      <c r="AC10" s="29">
         <v>0.71584070796460164</v>
       </c>
     </row>
@@ -12275,6 +12348,56 @@
     <mergeCell ref="N1:Q1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B10">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color theme="7"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C10">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color theme="7"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D10">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color theme="7"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E10">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color theme="7"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F10">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color theme="7"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G10">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -12284,7 +12407,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C10">
+  <conditionalFormatting sqref="H3:H10">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -12294,7 +12417,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D10">
+  <conditionalFormatting sqref="I3:I10">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -12304,7 +12427,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E10">
+  <conditionalFormatting sqref="J3:J10">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -12314,7 +12437,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F10">
+  <conditionalFormatting sqref="K3:K10">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -12324,7 +12447,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G10">
+  <conditionalFormatting sqref="L3:L10">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -12334,7 +12457,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H10">
+  <conditionalFormatting sqref="M3:M10">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -12344,7 +12467,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I10">
+  <conditionalFormatting sqref="N3:N10">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -12354,7 +12477,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J10">
+  <conditionalFormatting sqref="O3:O10">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -12364,7 +12487,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K10">
+  <conditionalFormatting sqref="P3:P10">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -12374,7 +12497,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L10">
+  <conditionalFormatting sqref="Q3:Q10">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -12384,7 +12507,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M10">
+  <conditionalFormatting sqref="R3:R10">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -12394,7 +12517,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N10">
+  <conditionalFormatting sqref="S3:S10">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -12404,7 +12527,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O10">
+  <conditionalFormatting sqref="T3:T10">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -12414,7 +12537,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P10">
+  <conditionalFormatting sqref="U3:U10">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -12424,7 +12547,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q10">
+  <conditionalFormatting sqref="V3:V10">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -12434,7 +12557,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R3:R10">
+  <conditionalFormatting sqref="W3:W10">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -12444,7 +12567,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S10">
+  <conditionalFormatting sqref="X3:X10">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -12454,7 +12577,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T3:T10">
+  <conditionalFormatting sqref="Y3:Y10">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -12464,95 +12587,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U3:U10">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="0"/>
-        <color theme="7"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V10">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="0"/>
-        <color theme="7"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W3:W10">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="0"/>
-        <color theme="7"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X3:X10">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="0"/>
-        <color theme="7"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y10">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="0"/>
-        <color theme="7"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="Z3:Z10">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="0"/>
-        <color theme="7"/>
-      </colorScale>
-    </cfRule>
+    <cfRule type="top10" dxfId="3" priority="4" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA3:AA10">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="0"/>
-        <color theme="7"/>
-      </colorScale>
-    </cfRule>
+    <cfRule type="top10" dxfId="2" priority="3" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB3:AB10">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="0"/>
-        <color theme="7"/>
-      </colorScale>
-    </cfRule>
+    <cfRule type="top10" dxfId="1" priority="2" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC3:AC10">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="0"/>
-        <color theme="7"/>
-      </colorScale>
-    </cfRule>
+    <cfRule type="top10" dxfId="0" priority="1" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>